<commit_message>
msz - mandatory fields checks part 2
</commit_message>
<xml_diff>
--- a/Data/Pages/dlgAutomobileInsurance_pagVehicleData.xlsx
+++ b/Data/Pages/dlgAutomobileInsurance_pagVehicleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9741DDFE-6B0C-4982-80EB-11B8C80CF3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125DB304-50AE-462B-BFCA-D7230EB38162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3132" yWindow="3096" windowWidth="32112" windowHeight="11364" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="3432" yWindow="4152" windowWidth="32112" windowHeight="11364" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -63,33 +63,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>id=make</t>
-  </si>
-  <si>
-    <t>id=engineperformance</t>
-  </si>
-  <si>
-    <t>id=dateofmanufacture</t>
-  </si>
-  <si>
-    <t>id=numberofseats</t>
-  </si>
-  <si>
-    <t>id=fuel</t>
-  </si>
-  <si>
-    <t>id=listprice</t>
-  </si>
-  <si>
-    <t>id=licenseplatenumber</t>
-  </si>
-  <si>
-    <t>id=annualmileage</t>
-  </si>
-  <si>
-    <t>id=nextenterinsurantdata</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -148,6 +121,33 @@
   </si>
   <si>
     <t>&lt;FilledMandatoryField&gt;</t>
+  </si>
+  <si>
+    <t>//*[@id='make']</t>
+  </si>
+  <si>
+    <t>//*[@id='engineperformance']</t>
+  </si>
+  <si>
+    <t>//*[@id='dateofmanufacture']</t>
+  </si>
+  <si>
+    <t>//*[@id='numberofseats']</t>
+  </si>
+  <si>
+    <t>//*[@id='fuel']</t>
+  </si>
+  <si>
+    <t>//*[@id='listprice']</t>
+  </si>
+  <si>
+    <t>//*[@id='licenseplatenumber']</t>
+  </si>
+  <si>
+    <t>//*[@id='annualmileage']</t>
+  </si>
+  <si>
+    <t>//*[@id='nextenterinsurantdata']</t>
   </si>
 </sst>
 </file>
@@ -235,8 +235,8 @@
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1352964</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>255684</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
@@ -573,15 +573,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="84" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="8" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.77734375" style="1" bestFit="1" customWidth="1"/>
@@ -593,34 +595,34 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -642,10 +644,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -654,10 +656,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>4</v>
@@ -674,7 +676,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>11</v>
@@ -696,7 +698,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
@@ -705,22 +707,22 @@
         <v>100</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>11</v>
@@ -728,39 +730,39 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
@@ -768,34 +770,34 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>